<commit_message>
- fixed NPE and failed tests
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/localdb/artifact/plan/crawl_and_search.xlsx
+++ b/examples/localdb/artifact/plan/crawl_and_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/localdb/artifact/plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6C0267-C725-6C4F-8B78-25DE9BA0DFF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADC43E8-11FA-E34F-AEF8-80553F61B8B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="8580" windowWidth="32040" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25480" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -895,7 +895,7 @@
   <dimension ref="A1:N700"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>